<commit_message>
complete results for classification
</commit_message>
<xml_diff>
--- a/results/Comparison_correct.xlsx
+++ b/results/Comparison_correct.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29280" windowHeight="16640" tabRatio="991"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16600" tabRatio="991" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Regression" sheetId="1" r:id="rId1"/>
@@ -489,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
@@ -1244,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:T30"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1372,7 +1372,9 @@
       <c r="N8" t="s">
         <v>25</v>
       </c>
-      <c r="O8" s="1"/>
+      <c r="O8">
+        <v>0.67109043262032098</v>
+      </c>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.15">
       <c r="C9" s="8" t="s">
@@ -1515,6 +1517,9 @@
       <c r="F13" t="s">
         <v>25</v>
       </c>
+      <c r="G13">
+        <v>0.75017829900990096</v>
+      </c>
       <c r="K13" s="8" t="s">
         <v>31</v>
       </c>
@@ -1526,6 +1531,9 @@
       </c>
       <c r="N13" t="s">
         <v>25</v>
+      </c>
+      <c r="O13">
+        <v>0.82573259009900901</v>
       </c>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.15">
@@ -1546,7 +1554,7 @@
       </c>
       <c r="G14">
         <f>AVERAGE(G6:G13)</f>
-        <v>0.67455177271487521</v>
+        <v>0.68535556218559324</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>32</v>
@@ -1565,7 +1573,7 @@
       </c>
       <c r="O14">
         <f>AVERAGE(O6:O13)</f>
-        <v>0.80401680104483364</v>
+        <v>0.78812957542049966</v>
       </c>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.15">
@@ -1678,7 +1686,9 @@
       <c r="N24" t="s">
         <v>25</v>
       </c>
-      <c r="O24" s="1"/>
+      <c r="O24">
+        <v>7.0063683957219194E-2</v>
+      </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.15">
       <c r="C25" s="8" t="s">
@@ -1821,6 +1831,9 @@
       <c r="F29" t="s">
         <v>25</v>
       </c>
+      <c r="G29">
+        <v>0.11124575544554401</v>
+      </c>
       <c r="K29" s="8" t="s">
         <v>31</v>
       </c>
@@ -1832,6 +1845,9 @@
       </c>
       <c r="N29" t="s">
         <v>25</v>
+      </c>
+      <c r="O29">
+        <v>0.38538094950495</v>
       </c>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.15">
@@ -1852,7 +1868,7 @@
       </c>
       <c r="G30">
         <f>AVERAGE(G22:G29)</f>
-        <v>0.43252313209365484</v>
+        <v>0.38662636400106759</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>32</v>
@@ -1871,7 +1887,7 @@
       </c>
       <c r="O30">
         <f>AVERAGE(O22:O29)</f>
-        <v>0.63019023043664679</v>
+        <v>0.51519939794934333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>